<commit_message>
fix: implement export menu Fixes #7
</commit_message>
<xml_diff>
--- a/prisma/lcra-db.xlsx
+++ b/prisma/lcra-db.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BCBEFA-9DAA-CB4B-9EB3-F5BA60B4F7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315FB1CE-96EC-914A-89A5-B1656A68FF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
   <si>
     <t>Address</t>
   </si>
@@ -258,16 +258,51 @@
   </si>
   <si>
     <t>2023-06-11T16:00:00-04:00;2023-08-20T17:07:25-04:00</t>
+  </si>
+  <si>
+    <t>123 Adventure Drive</t>
+  </si>
+  <si>
+    <t>Adventure Drive</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>ksmith@email.com</t>
+  </si>
+  <si>
+    <t>2nd entry</t>
+  </si>
+  <si>
+    <t>Corn Roast</t>
+  </si>
+  <si>
+    <t>2023-06-11T16:00:00-04:00</t>
+  </si>
+  <si>
+    <t>cash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -290,13 +325,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -634,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG2"/>
+  <dimension ref="A1:BG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="BG1" sqref="BG1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -836,67 +874,31 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B2">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
+        <v>84</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
-      </c>
-      <c r="J2">
-        <v>4161234567</v>
-      </c>
-      <c r="K2">
-        <v>4162345678</v>
-      </c>
-      <c r="L2">
-        <v>4163456789</v>
-      </c>
-      <c r="M2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" t="s">
-        <v>73</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>4171234567</v>
-      </c>
-      <c r="U2" t="s">
-        <v>74</v>
-      </c>
-      <c r="V2" t="s">
-        <v>75</v>
-      </c>
-      <c r="W2" t="s">
-        <v>76</v>
       </c>
       <c r="AK2" t="s">
         <v>60</v>
@@ -905,7 +907,7 @@
         <v>77</v>
       </c>
       <c r="AM2" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="AN2">
         <v>0</v>
@@ -926,49 +928,165 @@
         <v>1</v>
       </c>
       <c r="AT2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="AU2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="AV2" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="AW2">
         <v>1</v>
       </c>
       <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>4161234567</v>
+      </c>
+      <c r="K3">
+        <v>4162345678</v>
+      </c>
+      <c r="L3">
+        <v>4163456789</v>
+      </c>
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>1</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="R3">
+        <v>4171234567</v>
+      </c>
+      <c r="U3" t="s">
+        <v>74</v>
+      </c>
+      <c r="V3" t="s">
+        <v>75</v>
+      </c>
+      <c r="W3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW3">
+        <v>1</v>
+      </c>
+      <c r="AX3">
+        <v>1</v>
+      </c>
+      <c r="AY3" t="s">
         <v>62</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="AZ3" t="s">
         <v>63</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BA3" t="s">
         <v>64</v>
       </c>
-      <c r="BB2">
-        <v>0</v>
-      </c>
-      <c r="BC2">
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
         <v>1</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BD3" t="s">
         <v>62</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BE3" t="s">
         <v>65</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BF3" t="s">
         <v>64</v>
       </c>
-      <c r="BG2">
+      <c r="BG3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{6B4B139F-5BD3-0642-96FD-B1E293BB7330}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: implement export menu (#17)
</commit_message>
<xml_diff>
--- a/prisma/lcra-db.xlsx
+++ b/prisma/lcra-db.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BCBEFA-9DAA-CB4B-9EB3-F5BA60B4F7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315FB1CE-96EC-914A-89A5-B1656A68FF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
   <si>
     <t>Address</t>
   </si>
@@ -258,16 +258,51 @@
   </si>
   <si>
     <t>2023-06-11T16:00:00-04:00;2023-08-20T17:07:25-04:00</t>
+  </si>
+  <si>
+    <t>123 Adventure Drive</t>
+  </si>
+  <si>
+    <t>Adventure Drive</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>ksmith@email.com</t>
+  </si>
+  <si>
+    <t>2nd entry</t>
+  </si>
+  <si>
+    <t>Corn Roast</t>
+  </si>
+  <si>
+    <t>2023-06-11T16:00:00-04:00</t>
+  </si>
+  <si>
+    <t>cash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -290,13 +325,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -634,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG2"/>
+  <dimension ref="A1:BG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="BG1" sqref="BG1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -836,67 +874,31 @@
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B2">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
+        <v>84</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
-      </c>
-      <c r="J2">
-        <v>4161234567</v>
-      </c>
-      <c r="K2">
-        <v>4162345678</v>
-      </c>
-      <c r="L2">
-        <v>4163456789</v>
-      </c>
-      <c r="M2" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" t="s">
-        <v>73</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>4171234567</v>
-      </c>
-      <c r="U2" t="s">
-        <v>74</v>
-      </c>
-      <c r="V2" t="s">
-        <v>75</v>
-      </c>
-      <c r="W2" t="s">
-        <v>76</v>
       </c>
       <c r="AK2" t="s">
         <v>60</v>
@@ -905,7 +907,7 @@
         <v>77</v>
       </c>
       <c r="AM2" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="AN2">
         <v>0</v>
@@ -926,49 +928,165 @@
         <v>1</v>
       </c>
       <c r="AT2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="AU2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="AV2" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="AW2">
         <v>1</v>
       </c>
       <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>4161234567</v>
+      </c>
+      <c r="K3">
+        <v>4162345678</v>
+      </c>
+      <c r="L3">
+        <v>4163456789</v>
+      </c>
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>1</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="R3">
+        <v>4171234567</v>
+      </c>
+      <c r="U3" t="s">
+        <v>74</v>
+      </c>
+      <c r="V3" t="s">
+        <v>75</v>
+      </c>
+      <c r="W3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW3">
+        <v>1</v>
+      </c>
+      <c r="AX3">
+        <v>1</v>
+      </c>
+      <c r="AY3" t="s">
         <v>62</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="AZ3" t="s">
         <v>63</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BA3" t="s">
         <v>64</v>
       </c>
-      <c r="BB2">
-        <v>0</v>
-      </c>
-      <c r="BC2">
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
         <v>1</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BD3" t="s">
         <v>62</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BE3" t="s">
         <v>65</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BF3" t="s">
         <v>64</v>
       </c>
-      <c r="BG2">
+      <c r="BG3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{6B4B139F-5BD3-0642-96FD-B1E293BB7330}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: add eventlist property to community Fixes #16
</commit_message>
<xml_diff>
--- a/prisma/lcra-db.xlsx
+++ b/prisma/lcra-db.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315FB1CE-96EC-914A-89A5-B1656A68FF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC86CE7B-EF0D-FA4A-A3F7-5A4DD1448718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -281,10 +281,10 @@
     <t>Corn Roast</t>
   </si>
   <si>
-    <t>2023-06-11T16:00:00-04:00</t>
-  </si>
-  <si>
     <t>cash</t>
+  </si>
+  <si>
+    <t>2023-08-20T17:07:25-04:00</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -691,6 +691,9 @@
     <col min="37" max="37" width="19.6640625" customWidth="1"/>
     <col min="38" max="38" width="16" customWidth="1"/>
     <col min="39" max="39" width="40" customWidth="1"/>
+    <col min="46" max="46" width="27.6640625" customWidth="1"/>
+    <col min="47" max="47" width="47" customWidth="1"/>
+    <col min="57" max="57" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.2">
@@ -931,10 +934,10 @@
         <v>87</v>
       </c>
       <c r="AU2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AV2" t="s">
         <v>88</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>89</v>
       </c>
       <c r="AW2">
         <v>1</v>

</xml_diff>

<commit_message>
fix: implement dashboard (#18)
</commit_message>
<xml_diff>
--- a/prisma/lcra-db.xlsx
+++ b/prisma/lcra-db.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315FB1CE-96EC-914A-89A5-B1656A68FF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC86CE7B-EF0D-FA4A-A3F7-5A4DD1448718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -281,10 +281,10 @@
     <t>Corn Roast</t>
   </si>
   <si>
-    <t>2023-06-11T16:00:00-04:00</t>
-  </si>
-  <si>
     <t>cash</t>
+  </si>
+  <si>
+    <t>2023-08-20T17:07:25-04:00</t>
   </si>
 </sst>
 </file>
@@ -674,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -691,6 +691,9 @@
     <col min="37" max="37" width="19.6640625" customWidth="1"/>
     <col min="38" max="38" width="16" customWidth="1"/>
     <col min="39" max="39" width="40" customWidth="1"/>
+    <col min="46" max="46" width="27.6640625" customWidth="1"/>
+    <col min="47" max="47" width="47" customWidth="1"/>
+    <col min="57" max="57" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.2">
@@ -931,10 +934,10 @@
         <v>87</v>
       </c>
       <c r="AU2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AV2" t="s">
         <v>88</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>89</v>
       </c>
       <c r="AW2">
         <v>1</v>

</xml_diff>

<commit_message>
refactor: consolidate app path into app-path function
</commit_message>
<xml_diff>
--- a/prisma/lcra-db.xlsx
+++ b/prisma/lcra-db.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC86CE7B-EF0D-FA4A-A3F7-5A4DD1448718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6681BCE3-6BA5-7243-B598-4E989D2550DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>Address</t>
   </si>
@@ -675,7 +675,7 @@
   <dimension ref="A1:BG3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2"/>
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1019,9 +1019,6 @@
       <c r="AK3" t="s">
         <v>60</v>
       </c>
-      <c r="AL3" t="s">
-        <v>77</v>
-      </c>
       <c r="AM3" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
fix: refactor API for giving access to a community (#26)
</commit_message>
<xml_diff>
--- a/prisma/lcra-db.xlsx
+++ b/prisma/lcra-db.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC86CE7B-EF0D-FA4A-A3F7-5A4DD1448718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6681BCE3-6BA5-7243-B598-4E989D2550DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>Address</t>
   </si>
@@ -675,7 +675,7 @@
   <dimension ref="A1:BG3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2"/>
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1019,9 +1019,6 @@
       <c r="AK3" t="s">
         <v>60</v>
       </c>
-      <c r="AL3" t="s">
-        <v>77</v>
-      </c>
       <c r="AM3" t="s">
         <v>38</v>
       </c>

</xml_diff>